<commit_message>
validated/updated eruption dataset date
</commit_message>
<xml_diff>
--- a/data/eruptions_recent.xlsx
+++ b/data/eruptions_recent.xlsx
@@ -398,10 +398,10 @@
         <v>44341.0</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>45487.0</v>
+        <v>45490.0</v>
       </c>
       <c r="D13" t="n">
-        <v>1146.0</v>
+        <v>1149.0</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
updated datasets to include some unconmfirmed eruptions
</commit_message>
<xml_diff>
--- a/data/eruptions_recent.xlsx
+++ b/data/eruptions_recent.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="32">
   <si>
     <t>volcano</t>
   </si>
@@ -101,7 +101,13 @@
     <t>St. Helens</t>
   </si>
   <si>
+    <t>Wrangell</t>
+  </si>
+  <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -190,7 +196,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F2"/>
     </row>
@@ -208,7 +214,7 @@
         <v>0.0</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3"/>
     </row>
@@ -226,7 +232,7 @@
         <v>86.0</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4"/>
     </row>
@@ -244,7 +250,7 @@
         <v>0.0</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" t="n">
         <v>1.0</v>
@@ -264,7 +270,7 @@
         <v>1.0</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" t="n">
         <v>1.0</v>
@@ -284,7 +290,7 @@
         <v>115.0</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" t="n">
         <v>3.0</v>
@@ -304,7 +310,7 @@
         <v>13.0</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F8" t="n">
         <v>0.0</v>
@@ -324,7 +330,7 @@
         <v>205.0</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F9" t="n">
         <v>1.0</v>
@@ -344,7 +350,7 @@
         <v>717.0</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" t="n">
         <v>0.0</v>
@@ -364,7 +370,7 @@
         <v>489.0</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" t="n">
         <v>2.0</v>
@@ -384,7 +390,7 @@
         <v>39.0</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" t="n">
         <v>2.0</v>
@@ -398,13 +404,13 @@
         <v>44341.0</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>45490.0</v>
+        <v>45491.0</v>
       </c>
       <c r="D13" t="n">
-        <v>1149.0</v>
+        <v>1150.0</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F13" t="n">
         <v>2.0</v>
@@ -424,7 +430,7 @@
         <v>36.0</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" t="n">
         <v>1.0</v>
@@ -444,7 +450,7 @@
         <v>822.0</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F15" t="n">
         <v>2.0</v>
@@ -464,7 +470,7 @@
         <v>154.0</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F16" t="n">
         <v>0.0</v>
@@ -484,7 +490,7 @@
         <v>0.0</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F17" t="n">
         <v>3.0</v>
@@ -504,7 +510,7 @@
         <v>195.0</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F18" t="n">
         <v>1.0</v>
@@ -512,59 +518,57 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B19" t="n" s="2">
-        <v>43669.0</v>
+        <v>43776.0</v>
       </c>
       <c r="C19" t="n" s="2">
-        <v>43955.0</v>
+        <v>43806.0</v>
       </c>
       <c r="D19" t="n">
-        <v>286.0</v>
+        <v>30.0</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" t="n">
-        <v>3.0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B20" t="n" s="2">
-        <v>43662.0</v>
+        <v>43669.0</v>
       </c>
       <c r="C20" t="n" s="2">
-        <v>43701.0</v>
+        <v>43955.0</v>
       </c>
       <c r="D20" t="n">
-        <v>39.0</v>
+        <v>286.0</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F20" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B21" t="n" s="2">
-        <v>43617.0</v>
+        <v>43662.0</v>
       </c>
       <c r="C21" t="n" s="2">
-        <v>43623.0</v>
+        <v>43701.0</v>
       </c>
       <c r="D21" t="n">
-        <v>6.0</v>
+        <v>39.0</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F21" t="n">
         <v>1.0</v>
@@ -572,19 +576,19 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B22" t="n" s="2">
-        <v>43351.0</v>
+        <v>43617.0</v>
       </c>
       <c r="C22" t="n" s="2">
-        <v>43404.0</v>
+        <v>43623.0</v>
       </c>
       <c r="D22" t="n">
-        <v>53.0</v>
+        <v>6.0</v>
       </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F22" t="n">
         <v>1.0</v>
@@ -592,19 +596,19 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B23" t="n" s="2">
-        <v>43347.0</v>
+        <v>43351.0</v>
       </c>
       <c r="C23" t="n" s="2">
-        <v>43457.0</v>
+        <v>43404.0</v>
       </c>
       <c r="D23" t="n">
-        <v>110.0</v>
+        <v>53.0</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F23" t="n">
         <v>1.0</v>
@@ -612,19 +616,19 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B24" t="n" s="2">
-        <v>43261.0</v>
+        <v>43347.0</v>
       </c>
       <c r="C24" t="n" s="2">
-        <v>43323.0</v>
+        <v>43457.0</v>
       </c>
       <c r="D24" t="n">
-        <v>62.0</v>
+        <v>110.0</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F24" t="n">
         <v>1.0</v>
@@ -632,62 +636,62 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25" t="n" s="2">
-        <v>42724.0</v>
+        <v>43261.0</v>
       </c>
       <c r="C25" t="n" s="2">
-        <v>42977.0</v>
+        <v>43323.0</v>
       </c>
       <c r="D25" t="n">
-        <v>253.0</v>
+        <v>62.0</v>
       </c>
       <c r="E25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F25" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B26" t="n" s="2">
-        <v>42476.0</v>
+        <v>42724.0</v>
       </c>
       <c r="C26" t="n" s="2">
-        <v>43481.0</v>
+        <v>42977.0</v>
       </c>
       <c r="D26" t="n">
-        <v>1005.0</v>
+        <v>253.0</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F26" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B27" t="n" s="2">
-        <v>42456.0</v>
+        <v>42476.0</v>
       </c>
       <c r="C27" t="n" s="2">
-        <v>42581.0</v>
+        <v>43481.0</v>
       </c>
       <c r="D27" t="n">
-        <v>125.0</v>
+        <v>1005.0</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F27" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28">
@@ -695,16 +699,16 @@
         <v>13</v>
       </c>
       <c r="B28" t="n" s="2">
-        <v>41955.0</v>
+        <v>42456.0</v>
       </c>
       <c r="C28" t="n" s="2">
-        <v>41958.0</v>
+        <v>42581.0</v>
       </c>
       <c r="D28" t="n">
-        <v>3.0</v>
+        <v>125.0</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F28" t="n">
         <v>3.0</v>
@@ -715,16 +719,16 @@
         <v>13</v>
       </c>
       <c r="B29" t="n" s="2">
-        <v>41790.0</v>
+        <v>41955.0</v>
       </c>
       <c r="C29" t="n" s="2">
-        <v>41796.0</v>
+        <v>41958.0</v>
       </c>
       <c r="D29" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="E29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F29" t="n">
         <v>3.0</v>
@@ -732,79 +736,79 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B30" t="n" s="2">
-        <v>41753.0</v>
+        <v>41790.0</v>
       </c>
       <c r="C30" t="n" s="2">
-        <v>41776.0</v>
+        <v>41796.0</v>
       </c>
       <c r="D30" t="n">
-        <v>23.0</v>
+        <v>6.0</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F30" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B31" t="n" s="2">
-        <v>41669.0</v>
+        <v>41753.0</v>
       </c>
       <c r="C31" t="n" s="2">
-        <v>42188.0</v>
+        <v>41776.0</v>
       </c>
       <c r="D31" t="n">
-        <v>519.0</v>
+        <v>23.0</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F31" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B32" t="n" s="2">
-        <v>41438.0</v>
+        <v>41669.0</v>
       </c>
       <c r="C32" t="n" s="2">
-        <v>41559.0</v>
+        <v>42188.0</v>
       </c>
       <c r="D32" t="n">
-        <v>121.0</v>
+        <v>519.0</v>
       </c>
       <c r="E32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F32" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B33" t="n" s="2">
-        <v>41407.0</v>
+        <v>41438.0</v>
       </c>
       <c r="C33" t="n" s="2">
-        <v>41451.0</v>
+        <v>41559.0</v>
       </c>
       <c r="D33" t="n">
-        <v>44.0</v>
+        <v>121.0</v>
       </c>
       <c r="E33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F33" t="n">
         <v>3.0</v>
@@ -812,59 +816,59 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B34" t="n" s="2">
-        <v>41318.0</v>
+        <v>41407.0</v>
       </c>
       <c r="C34" t="n" s="2">
-        <v>42339.0</v>
+        <v>41451.0</v>
       </c>
       <c r="D34" t="n">
-        <v>1021.0</v>
+        <v>44.0</v>
       </c>
       <c r="E34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B35" t="n" s="2">
-        <v>41100.0</v>
+        <v>41318.0</v>
       </c>
       <c r="C35" t="n" s="2">
-        <v>41100.0</v>
+        <v>42339.0</v>
       </c>
       <c r="D35" t="n">
+        <v>1021.0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" t="n">
         <v>0.0</v>
-      </c>
-      <c r="E35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F35" t="n">
-        <v>2.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B36" t="n" s="2">
-        <v>40957.0</v>
+        <v>41100.0</v>
       </c>
       <c r="C36" t="n" s="2">
-        <v>40957.0</v>
+        <v>41100.0</v>
       </c>
       <c r="D36" t="n">
         <v>0.0</v>
       </c>
       <c r="E36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F36" t="n">
         <v>2.0</v>
@@ -872,19 +876,19 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B37" t="n" s="2">
-        <v>40743.0</v>
+        <v>40957.0</v>
       </c>
       <c r="C37" t="n" s="2">
-        <v>42234.0</v>
+        <v>40957.0</v>
       </c>
       <c r="D37" t="n">
-        <v>1491.0</v>
+        <v>0.0</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F37" t="n">
         <v>2.0</v>
@@ -892,19 +896,19 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B38" t="n" s="2">
-        <v>40656.0</v>
+        <v>40743.0</v>
       </c>
       <c r="C38" t="n" s="2">
-        <v>40787.0</v>
+        <v>42234.0</v>
       </c>
       <c r="D38" t="n">
-        <v>131.0</v>
+        <v>1491.0</v>
       </c>
       <c r="E38" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F38" t="n">
         <v>2.0</v>
@@ -912,19 +916,19 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B39" t="n" s="2">
-        <v>40328.0</v>
+        <v>40656.0</v>
       </c>
       <c r="C39" t="n" s="2">
-        <v>40331.0</v>
+        <v>40787.0</v>
       </c>
       <c r="D39" t="n">
-        <v>3.0</v>
+        <v>131.0</v>
       </c>
       <c r="E39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F39" t="n">
         <v>2.0</v>
@@ -932,102 +936,100 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B40" t="n" s="2">
-        <v>40325.0</v>
+        <v>40432.0</v>
       </c>
       <c r="C40" t="n" s="2">
-        <v>40327.0</v>
+        <v>40433.0</v>
       </c>
       <c r="D40" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E40" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" t="n">
-        <v>3.0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B41" t="n" s="2">
-        <v>40301.0</v>
+        <v>40328.0</v>
       </c>
       <c r="C41" t="n" s="2">
-        <v>40401.0</v>
+        <v>40331.0</v>
       </c>
       <c r="D41" t="n">
-        <v>100.0</v>
+        <v>3.0</v>
       </c>
       <c r="E41" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F41" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B42" t="n" s="2">
-        <v>40088.0</v>
+        <v>40325.0</v>
       </c>
       <c r="C42" t="n" s="2">
-        <v>40159.0</v>
+        <v>40327.0</v>
       </c>
       <c r="D42" t="n">
-        <v>71.0</v>
+        <v>2.0</v>
       </c>
       <c r="E42" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F42" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B43" t="n" s="2">
-        <v>39989.0</v>
+        <v>40301.0</v>
       </c>
       <c r="C43" t="n" s="2">
-        <v>39989.0</v>
+        <v>40401.0</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="E43" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F43" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B44" t="n" s="2">
-        <v>39887.0</v>
+        <v>40088.0</v>
       </c>
       <c r="C44" t="n" s="2">
-        <v>39995.0</v>
+        <v>40159.0</v>
       </c>
       <c r="D44" t="n">
-        <v>108.0</v>
+        <v>71.0</v>
       </c>
       <c r="E44" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F44" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="45">
@@ -1035,16 +1037,16 @@
         <v>18</v>
       </c>
       <c r="B45" t="n" s="2">
-        <v>39815.0</v>
+        <v>39989.0</v>
       </c>
       <c r="C45" t="n" s="2">
-        <v>39834.0</v>
+        <v>39989.0</v>
       </c>
       <c r="D45" t="n">
-        <v>19.0</v>
+        <v>0.0</v>
       </c>
       <c r="E45" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F45" t="n">
         <v>2.0</v>
@@ -1052,179 +1054,171 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B46" t="n" s="2">
-        <v>39667.0</v>
-      </c>
-      <c r="C46" t="n" s="2">
-        <v>39669.0</v>
-      </c>
-      <c r="D46" t="n">
-        <v>2.0</v>
-      </c>
+        <v>39918.0</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46"/>
       <c r="E46" t="s">
-        <v>29</v>
-      </c>
-      <c r="F46" t="n">
-        <v>4.0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F46"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B47" t="n" s="2">
-        <v>39641.0</v>
+        <v>39887.0</v>
       </c>
       <c r="C47" t="n" s="2">
-        <v>39679.0</v>
+        <v>39995.0</v>
       </c>
       <c r="D47" t="n">
-        <v>38.0</v>
+        <v>108.0</v>
       </c>
       <c r="E47" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F47" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B48" t="n" s="2">
-        <v>39500.0</v>
+        <v>39815.0</v>
       </c>
       <c r="C48" t="n" s="2">
-        <v>39508.0</v>
+        <v>39834.0</v>
       </c>
       <c r="D48" t="n">
-        <v>8.0</v>
+        <v>19.0</v>
       </c>
       <c r="E48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F48" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B49" t="n" s="2">
-        <v>39413.0</v>
+        <v>39667.0</v>
       </c>
       <c r="C49" t="n" s="2">
         <v>39669.0</v>
       </c>
       <c r="D49" t="n">
-        <v>256.0</v>
+        <v>2.0</v>
       </c>
       <c r="E49" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F49" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B50" t="n" s="2">
-        <v>39309.0</v>
+        <v>39641.0</v>
       </c>
       <c r="C50" t="n" s="2">
-        <v>39338.0</v>
+        <v>39679.0</v>
       </c>
       <c r="D50" t="n">
-        <v>29.0</v>
+        <v>38.0</v>
       </c>
       <c r="E50" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F50" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B51" t="n" s="2">
-        <v>39250.0</v>
+        <v>39500.0</v>
       </c>
       <c r="C51" t="n" s="2">
-        <v>39672.0</v>
+        <v>39508.0</v>
       </c>
       <c r="D51" t="n">
-        <v>422.0</v>
+        <v>8.0</v>
       </c>
       <c r="E51" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F51" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B52" t="n" s="2">
-        <v>39055.0</v>
+        <v>39490.0</v>
       </c>
       <c r="C52" t="n" s="2">
-        <v>39059.0</v>
+        <v>39490.0</v>
       </c>
       <c r="D52" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="E52" t="s">
-        <v>29</v>
-      </c>
-      <c r="F52" t="n">
-        <v>1.0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F52"/>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B53" t="n" s="2">
-        <v>39046.0</v>
+        <v>39413.0</v>
       </c>
       <c r="C53" t="n" s="2">
-        <v>39144.0</v>
+        <v>39669.0</v>
       </c>
       <c r="D53" t="n">
-        <v>98.0</v>
+        <v>256.0</v>
       </c>
       <c r="E53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F53" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B54" t="n" s="2">
-        <v>38977.0</v>
+        <v>39309.0</v>
       </c>
       <c r="C54" t="n" s="2">
-        <v>38977.0</v>
+        <v>39338.0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0</v>
+        <v>29.0</v>
       </c>
       <c r="E54" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F54" t="n">
         <v>2.0</v>
@@ -1232,19 +1226,19 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B55" t="n" s="2">
-        <v>38796.0</v>
+        <v>39250.0</v>
       </c>
       <c r="C55" t="n" s="2">
-        <v>38894.0</v>
+        <v>39672.0</v>
       </c>
       <c r="D55" t="n">
-        <v>98.0</v>
+        <v>422.0</v>
       </c>
       <c r="E55" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F55" t="n">
         <v>2.0</v>
@@ -1252,19 +1246,19 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B56" t="n" s="2">
-        <v>38779.0</v>
+        <v>39055.0</v>
       </c>
       <c r="C56" t="n" s="2">
-        <v>38967.0</v>
+        <v>39059.0</v>
       </c>
       <c r="D56" t="n">
-        <v>188.0</v>
+        <v>4.0</v>
       </c>
       <c r="E56" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F56" t="n">
         <v>1.0</v>
@@ -1272,195 +1266,199 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B57" t="n" s="2">
-        <v>38754.0</v>
+        <v>39046.0</v>
       </c>
       <c r="C57" t="n" s="2">
-        <v>39018.0</v>
+        <v>39144.0</v>
       </c>
       <c r="D57" t="n">
-        <v>264.0</v>
+        <v>98.0</v>
       </c>
       <c r="E57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F57" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B58" t="n" s="2">
-        <v>38695.0</v>
+        <v>38977.0</v>
       </c>
       <c r="C58" t="n" s="2">
-        <v>38834.0</v>
+        <v>38977.0</v>
       </c>
       <c r="D58" t="n">
-        <v>139.0</v>
+        <v>0.0</v>
       </c>
       <c r="E58" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F58" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B59" t="n" s="2">
-        <v>38602.0</v>
+        <v>38796.0</v>
       </c>
       <c r="C59" t="n" s="2">
-        <v>38660.0</v>
+        <v>38894.0</v>
       </c>
       <c r="D59" t="n">
-        <v>58.0</v>
+        <v>98.0</v>
       </c>
       <c r="E59" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F59" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B60" t="n" s="2">
-        <v>38424.0</v>
+        <v>38779.0</v>
       </c>
       <c r="C60" t="n" s="2">
-        <v>38683.0</v>
+        <v>38967.0</v>
       </c>
       <c r="D60" t="n">
-        <v>259.0</v>
+        <v>188.0</v>
       </c>
       <c r="E60" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F60" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B61" t="n" s="2">
-        <v>38406.0</v>
+        <v>38754.0</v>
       </c>
       <c r="C61" t="n" s="2">
-        <v>38477.0</v>
+        <v>39018.0</v>
       </c>
       <c r="D61" t="n">
-        <v>71.0</v>
+        <v>264.0</v>
       </c>
       <c r="E61" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F61" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B62" t="n" s="2">
-        <v>38356.0</v>
+        <v>38695.0</v>
       </c>
       <c r="C62" t="n" s="2">
-        <v>38397.0</v>
+        <v>38834.0</v>
       </c>
       <c r="D62" t="n">
-        <v>41.0</v>
+        <v>139.0</v>
       </c>
       <c r="E62" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F62" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B63" t="n" s="2">
-        <v>38261.0</v>
+        <v>38602.0</v>
       </c>
       <c r="C63" t="n" s="2">
-        <v>39474.0</v>
+        <v>38660.0</v>
       </c>
       <c r="D63" t="n">
-        <v>1213.0</v>
+        <v>58.0</v>
       </c>
       <c r="E63" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F63" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B64" t="n" s="2">
-        <v>38172.0</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64"/>
+        <v>38424.0</v>
+      </c>
+      <c r="C64" t="n" s="2">
+        <v>38683.0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>259.0</v>
+      </c>
       <c r="E64" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F64" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B65" t="n" s="2">
-        <v>38089.0</v>
+        <v>38406.0</v>
       </c>
       <c r="C65" t="n" s="2">
-        <v>38598.0</v>
+        <v>38477.0</v>
       </c>
       <c r="D65" t="n">
-        <v>509.0</v>
+        <v>71.0</v>
       </c>
       <c r="E65" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F65" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B66" t="n" s="2">
-        <v>38034.0</v>
+        <v>38356.0</v>
       </c>
       <c r="C66" t="n" s="2">
-        <v>38184.0</v>
+        <v>38397.0</v>
       </c>
       <c r="D66" t="n">
-        <v>150.0</v>
+        <v>41.0</v>
       </c>
       <c r="E66" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F66" t="n">
         <v>2.0</v>
@@ -1468,19 +1466,19 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B67" t="n" s="2">
-        <v>38033.0</v>
+        <v>38261.0</v>
       </c>
       <c r="C67" t="n" s="2">
-        <v>38235.0</v>
+        <v>39474.0</v>
       </c>
       <c r="D67" t="n">
-        <v>202.0</v>
+        <v>1213.0</v>
       </c>
       <c r="E67" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F67" t="n">
         <v>2.0</v>
@@ -1488,97 +1486,205 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B68" t="n" s="2">
-        <v>37751.0</v>
-      </c>
-      <c r="C68" t="n" s="2">
-        <v>37814.0</v>
-      </c>
-      <c r="D68" t="n">
-        <v>63.0</v>
-      </c>
+        <v>38172.0</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68"/>
       <c r="E68" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F68" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B69" t="n" s="2">
-        <v>37523.0</v>
+        <v>38089.0</v>
       </c>
       <c r="C69" t="n" s="2">
-        <v>37703.0</v>
+        <v>38598.0</v>
       </c>
       <c r="D69" t="n">
-        <v>180.0</v>
+        <v>509.0</v>
       </c>
       <c r="E69" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F69" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B70" t="n" s="2">
-        <v>37453.0</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70"/>
+        <v>38034.0</v>
+      </c>
+      <c r="C70" t="n" s="2">
+        <v>38184.0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>150.0</v>
+      </c>
       <c r="E70" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F70" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B71" t="n" s="2">
-        <v>37005.0</v>
+        <v>38033.0</v>
       </c>
       <c r="C71" t="n" s="2">
-        <v>37006.0</v>
+        <v>38235.0</v>
       </c>
       <c r="D71" t="n">
-        <v>1.0</v>
+        <v>202.0</v>
       </c>
       <c r="E71" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F71" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72" t="n" s="2">
+        <v>37751.0</v>
+      </c>
+      <c r="C72" t="n" s="2">
+        <v>37814.0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>30</v>
+      </c>
+      <c r="F72" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" t="n" s="2">
+        <v>37523.0</v>
+      </c>
+      <c r="C73" t="n" s="2">
+        <v>37703.0</v>
+      </c>
+      <c r="D73" t="n">
+        <v>180.0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>30</v>
+      </c>
+      <c r="F73" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>29</v>
+      </c>
+      <c r="B74" t="n" s="2">
+        <v>37469.0</v>
+      </c>
+      <c r="C74" t="n" s="2">
+        <v>37470.0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>31</v>
+      </c>
+      <c r="F74"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" t="n" s="2">
+        <v>37453.0</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75"/>
+      <c r="E75" t="s">
+        <v>30</v>
+      </c>
+      <c r="F75" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" t="n" s="2">
+        <v>37047.0</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76"/>
+      <c r="E76" t="s">
+        <v>31</v>
+      </c>
+      <c r="F76"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" t="n" s="2">
+        <v>37005.0</v>
+      </c>
+      <c r="C77" t="n" s="2">
+        <v>37006.0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>30</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
         <v>18</v>
       </c>
-      <c r="B72" t="n" s="2">
+      <c r="B78" t="n" s="2">
         <v>36924.0</v>
       </c>
-      <c r="C72" t="n" s="2">
+      <c r="C78" t="n" s="2">
         <v>36996.0</v>
       </c>
-      <c r="D72" t="n">
+      <c r="D78" t="n">
         <v>72.0</v>
       </c>
-      <c r="E72" t="s">
-        <v>29</v>
-      </c>
-      <c r="F72" t="n">
+      <c r="E78" t="s">
+        <v>30</v>
+      </c>
+      <c r="F78" t="n">
         <v>3.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated data files (see previous commit)
</commit_message>
<xml_diff>
--- a/data/eruptions_recent.xlsx
+++ b/data/eruptions_recent.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="32">
   <si>
     <t>volcano</t>
   </si>
@@ -404,10 +404,10 @@
         <v>44341.0</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>45491.0</v>
+        <v>45492.0</v>
       </c>
       <c r="D13" t="n">
-        <v>1150.0</v>
+        <v>1151.0</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
@@ -1054,70 +1054,76 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B46" t="n" s="2">
-        <v>39918.0</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46"/>
+        <v>39887.0</v>
+      </c>
+      <c r="C46" t="n" s="2">
+        <v>39995.0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>108.0</v>
+      </c>
       <c r="E46" t="s">
-        <v>31</v>
-      </c>
-      <c r="F46"/>
+        <v>30</v>
+      </c>
+      <c r="F46" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B47" t="n" s="2">
-        <v>39887.0</v>
+        <v>39815.0</v>
       </c>
       <c r="C47" t="n" s="2">
-        <v>39995.0</v>
+        <v>39834.0</v>
       </c>
       <c r="D47" t="n">
-        <v>108.0</v>
+        <v>19.0</v>
       </c>
       <c r="E47" t="s">
         <v>30</v>
       </c>
       <c r="F47" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B48" t="n" s="2">
-        <v>39815.0</v>
+        <v>39667.0</v>
       </c>
       <c r="C48" t="n" s="2">
-        <v>39834.0</v>
+        <v>39669.0</v>
       </c>
       <c r="D48" t="n">
-        <v>19.0</v>
+        <v>2.0</v>
       </c>
       <c r="E48" t="s">
         <v>30</v>
       </c>
       <c r="F48" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B49" t="n" s="2">
-        <v>39667.0</v>
+        <v>39641.0</v>
       </c>
       <c r="C49" t="n" s="2">
-        <v>39669.0</v>
+        <v>39679.0</v>
       </c>
       <c r="D49" t="n">
-        <v>2.0</v>
+        <v>38.0</v>
       </c>
       <c r="E49" t="s">
         <v>30</v>
@@ -1128,74 +1134,74 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B50" t="n" s="2">
-        <v>39641.0</v>
+        <v>39500.0</v>
       </c>
       <c r="C50" t="n" s="2">
-        <v>39679.0</v>
+        <v>39508.0</v>
       </c>
       <c r="D50" t="n">
-        <v>38.0</v>
+        <v>8.0</v>
       </c>
       <c r="E50" t="s">
         <v>30</v>
       </c>
       <c r="F50" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B51" t="n" s="2">
-        <v>39500.0</v>
+        <v>39490.0</v>
       </c>
       <c r="C51" t="n" s="2">
-        <v>39508.0</v>
+        <v>39490.0</v>
       </c>
       <c r="D51" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="E51" t="s">
-        <v>30</v>
-      </c>
-      <c r="F51" t="n">
-        <v>1.0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B52" t="n" s="2">
-        <v>39490.0</v>
+        <v>39413.0</v>
       </c>
       <c r="C52" t="n" s="2">
-        <v>39490.0</v>
+        <v>39669.0</v>
       </c>
       <c r="D52" t="n">
-        <v>0.0</v>
+        <v>256.0</v>
       </c>
       <c r="E52" t="s">
-        <v>31</v>
-      </c>
-      <c r="F52"/>
+        <v>30</v>
+      </c>
+      <c r="F52" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B53" t="n" s="2">
-        <v>39413.0</v>
+        <v>39309.0</v>
       </c>
       <c r="C53" t="n" s="2">
-        <v>39669.0</v>
+        <v>39338.0</v>
       </c>
       <c r="D53" t="n">
-        <v>256.0</v>
+        <v>29.0</v>
       </c>
       <c r="E53" t="s">
         <v>30</v>
@@ -1206,16 +1212,16 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B54" t="n" s="2">
-        <v>39309.0</v>
+        <v>39250.0</v>
       </c>
       <c r="C54" t="n" s="2">
-        <v>39338.0</v>
+        <v>39672.0</v>
       </c>
       <c r="D54" t="n">
-        <v>29.0</v>
+        <v>422.0</v>
       </c>
       <c r="E54" t="s">
         <v>30</v>
@@ -1226,36 +1232,36 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B55" t="n" s="2">
-        <v>39250.0</v>
+        <v>39055.0</v>
       </c>
       <c r="C55" t="n" s="2">
-        <v>39672.0</v>
+        <v>39059.0</v>
       </c>
       <c r="D55" t="n">
-        <v>422.0</v>
+        <v>4.0</v>
       </c>
       <c r="E55" t="s">
         <v>30</v>
       </c>
       <c r="F55" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B56" t="n" s="2">
-        <v>39055.0</v>
+        <v>39046.0</v>
       </c>
       <c r="C56" t="n" s="2">
-        <v>39059.0</v>
+        <v>39144.0</v>
       </c>
       <c r="D56" t="n">
-        <v>4.0</v>
+        <v>98.0</v>
       </c>
       <c r="E56" t="s">
         <v>30</v>
@@ -1266,36 +1272,36 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B57" t="n" s="2">
-        <v>39046.0</v>
+        <v>38977.0</v>
       </c>
       <c r="C57" t="n" s="2">
-        <v>39144.0</v>
+        <v>38977.0</v>
       </c>
       <c r="D57" t="n">
-        <v>98.0</v>
+        <v>0.0</v>
       </c>
       <c r="E57" t="s">
         <v>30</v>
       </c>
       <c r="F57" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B58" t="n" s="2">
-        <v>38977.0</v>
+        <v>38796.0</v>
       </c>
       <c r="C58" t="n" s="2">
-        <v>38977.0</v>
+        <v>38894.0</v>
       </c>
       <c r="D58" t="n">
-        <v>0.0</v>
+        <v>98.0</v>
       </c>
       <c r="E58" t="s">
         <v>30</v>
@@ -1306,56 +1312,56 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B59" t="n" s="2">
-        <v>38796.0</v>
+        <v>38779.0</v>
       </c>
       <c r="C59" t="n" s="2">
-        <v>38894.0</v>
+        <v>38967.0</v>
       </c>
       <c r="D59" t="n">
-        <v>98.0</v>
+        <v>188.0</v>
       </c>
       <c r="E59" t="s">
         <v>30</v>
       </c>
       <c r="F59" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B60" t="n" s="2">
-        <v>38779.0</v>
+        <v>38754.0</v>
       </c>
       <c r="C60" t="n" s="2">
-        <v>38967.0</v>
+        <v>39018.0</v>
       </c>
       <c r="D60" t="n">
-        <v>188.0</v>
+        <v>264.0</v>
       </c>
       <c r="E60" t="s">
         <v>30</v>
       </c>
       <c r="F60" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B61" t="n" s="2">
-        <v>38754.0</v>
+        <v>38695.0</v>
       </c>
       <c r="C61" t="n" s="2">
-        <v>39018.0</v>
+        <v>38834.0</v>
       </c>
       <c r="D61" t="n">
-        <v>264.0</v>
+        <v>139.0</v>
       </c>
       <c r="E61" t="s">
         <v>30</v>
@@ -1366,96 +1372,96 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B62" t="n" s="2">
-        <v>38695.0</v>
+        <v>38602.0</v>
       </c>
       <c r="C62" t="n" s="2">
-        <v>38834.0</v>
+        <v>38660.0</v>
       </c>
       <c r="D62" t="n">
-        <v>139.0</v>
+        <v>58.0</v>
       </c>
       <c r="E62" t="s">
         <v>30</v>
       </c>
       <c r="F62" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B63" t="n" s="2">
-        <v>38602.0</v>
+        <v>38424.0</v>
       </c>
       <c r="C63" t="n" s="2">
-        <v>38660.0</v>
+        <v>38683.0</v>
       </c>
       <c r="D63" t="n">
-        <v>58.0</v>
+        <v>259.0</v>
       </c>
       <c r="E63" t="s">
         <v>30</v>
       </c>
       <c r="F63" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B64" t="n" s="2">
-        <v>38424.0</v>
+        <v>38406.0</v>
       </c>
       <c r="C64" t="n" s="2">
-        <v>38683.0</v>
+        <v>38477.0</v>
       </c>
       <c r="D64" t="n">
-        <v>259.0</v>
+        <v>71.0</v>
       </c>
       <c r="E64" t="s">
         <v>30</v>
       </c>
       <c r="F64" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B65" t="n" s="2">
-        <v>38406.0</v>
+        <v>38356.0</v>
       </c>
       <c r="C65" t="n" s="2">
-        <v>38477.0</v>
+        <v>38397.0</v>
       </c>
       <c r="D65" t="n">
-        <v>71.0</v>
+        <v>41.0</v>
       </c>
       <c r="E65" t="s">
         <v>30</v>
       </c>
       <c r="F65" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B66" t="n" s="2">
-        <v>38356.0</v>
+        <v>38261.0</v>
       </c>
       <c r="C66" t="n" s="2">
-        <v>38397.0</v>
+        <v>39474.0</v>
       </c>
       <c r="D66" t="n">
-        <v>41.0</v>
+        <v>1213.0</v>
       </c>
       <c r="E66" t="s">
         <v>30</v>
@@ -1466,78 +1472,82 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B67" t="n" s="2">
-        <v>38261.0</v>
+        <v>38089.0</v>
       </c>
       <c r="C67" t="n" s="2">
-        <v>39474.0</v>
+        <v>38598.0</v>
       </c>
       <c r="D67" t="n">
-        <v>1213.0</v>
+        <v>509.0</v>
       </c>
       <c r="E67" t="s">
         <v>30</v>
       </c>
       <c r="F67" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B68" t="n" s="2">
-        <v>38172.0</v>
-      </c>
-      <c r="C68" s="2"/>
-      <c r="D68"/>
+        <v>38034.0</v>
+      </c>
+      <c r="C68" t="n" s="2">
+        <v>38184.0</v>
+      </c>
+      <c r="D68" t="n">
+        <v>150.0</v>
+      </c>
       <c r="E68" t="s">
         <v>30</v>
       </c>
       <c r="F68" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B69" t="n" s="2">
-        <v>38089.0</v>
+        <v>38033.0</v>
       </c>
       <c r="C69" t="n" s="2">
-        <v>38598.0</v>
+        <v>38235.0</v>
       </c>
       <c r="D69" t="n">
-        <v>509.0</v>
+        <v>202.0</v>
       </c>
       <c r="E69" t="s">
         <v>30</v>
       </c>
       <c r="F69" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B70" t="n" s="2">
-        <v>38034.0</v>
+        <v>37751.0</v>
       </c>
       <c r="C70" t="n" s="2">
-        <v>38184.0</v>
+        <v>37814.0</v>
       </c>
       <c r="D70" t="n">
-        <v>150.0</v>
+        <v>63.0</v>
       </c>
       <c r="E70" t="s">
         <v>30</v>
       </c>
       <c r="F70" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="71">
@@ -1545,146 +1555,76 @@
         <v>16</v>
       </c>
       <c r="B71" t="n" s="2">
-        <v>38033.0</v>
+        <v>37523.0</v>
       </c>
       <c r="C71" t="n" s="2">
-        <v>38235.0</v>
+        <v>37703.0</v>
       </c>
       <c r="D71" t="n">
-        <v>202.0</v>
+        <v>180.0</v>
       </c>
       <c r="E71" t="s">
         <v>30</v>
       </c>
       <c r="F71" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B72" t="n" s="2">
-        <v>37751.0</v>
+        <v>37469.0</v>
       </c>
       <c r="C72" t="n" s="2">
-        <v>37814.0</v>
+        <v>37470.0</v>
       </c>
       <c r="D72" t="n">
-        <v>63.0</v>
+        <v>1.0</v>
       </c>
       <c r="E72" t="s">
-        <v>30</v>
-      </c>
-      <c r="F72" t="n">
-        <v>3.0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F72"/>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B73" t="n" s="2">
-        <v>37523.0</v>
+        <v>37005.0</v>
       </c>
       <c r="C73" t="n" s="2">
-        <v>37703.0</v>
+        <v>37006.0</v>
       </c>
       <c r="D73" t="n">
-        <v>180.0</v>
+        <v>1.0</v>
       </c>
       <c r="E73" t="s">
         <v>30</v>
       </c>
       <c r="F73" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B74" t="n" s="2">
-        <v>37469.0</v>
+        <v>36924.0</v>
       </c>
       <c r="C74" t="n" s="2">
-        <v>37470.0</v>
+        <v>36996.0</v>
       </c>
       <c r="D74" t="n">
-        <v>1.0</v>
+        <v>72.0</v>
       </c>
       <c r="E74" t="s">
-        <v>31</v>
-      </c>
-      <c r="F74"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>7</v>
-      </c>
-      <c r="B75" t="n" s="2">
-        <v>37453.0</v>
-      </c>
-      <c r="C75" s="2"/>
-      <c r="D75"/>
-      <c r="E75" t="s">
-        <v>30</v>
-      </c>
-      <c r="F75" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>13</v>
-      </c>
-      <c r="B76" t="n" s="2">
-        <v>37047.0</v>
-      </c>
-      <c r="C76" s="2"/>
-      <c r="D76"/>
-      <c r="E76" t="s">
-        <v>31</v>
-      </c>
-      <c r="F76"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>8</v>
-      </c>
-      <c r="B77" t="n" s="2">
-        <v>37005.0</v>
-      </c>
-      <c r="C77" t="n" s="2">
-        <v>37006.0</v>
-      </c>
-      <c r="D77" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E77" t="s">
-        <v>30</v>
-      </c>
-      <c r="F77" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
-        <v>18</v>
-      </c>
-      <c r="B78" t="n" s="2">
-        <v>36924.0</v>
-      </c>
-      <c r="C78" t="n" s="2">
-        <v>36996.0</v>
-      </c>
-      <c r="D78" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="E78" t="s">
-        <v>30</v>
-      </c>
-      <c r="F78" t="n">
+        <v>30</v>
+      </c>
+      <c r="F74" t="n">
         <v>3.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix some volcano names for matching with other dataset
</commit_message>
<xml_diff>
--- a/data/eruptions_recent.xlsx
+++ b/data/eruptions_recent.xlsx
@@ -32,7 +32,7 @@
     <t>vei</t>
   </si>
   <si>
-    <t>Kilauea</t>
+    <t>Kīlauea</t>
   </si>
   <si>
     <t>Atka Volcanic Complex</t>
@@ -404,10 +404,10 @@
         <v>44341.0</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>45495.0</v>
+        <v>45496.0</v>
       </c>
       <c r="D13" t="n">
-        <v>1154.0</v>
+        <v>1155.0</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
tweak first example data frame to my liking (fewer NAs at top)
</commit_message>
<xml_diff>
--- a/data/eruptions_recent.xlsx
+++ b/data/eruptions_recent.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="32">
   <si>
     <t>volcano</t>
   </si>
@@ -32,12 +32,12 @@
     <t>vei</t>
   </si>
   <si>
+    <t>Kīlauea</t>
+  </si>
+  <si>
     <t>Atka Volcanic Complex</t>
   </si>
   <si>
-    <t>Kīlauea</t>
-  </si>
-  <si>
     <t>Ahyi</t>
   </si>
   <si>
@@ -59,16 +59,16 @@
     <t>Pagan</t>
   </si>
   <si>
+    <t>Veniaminof</t>
+  </si>
+  <si>
+    <t>Semisopochnoi</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
     <t>Great Sitkin</t>
-  </si>
-  <si>
-    <t>Veniaminof</t>
-  </si>
-  <si>
-    <t>Semisopochnoi</t>
-  </si>
-  <si>
-    <t>Cleveland</t>
   </si>
   <si>
     <t>Bogoslof</t>
@@ -187,13 +187,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="n" s="2">
-        <v>45708.0</v>
+        <v>45550.0</v>
       </c>
       <c r="C2" t="n" s="2">
-        <v>45825.0</v>
+        <v>45555.0</v>
       </c>
       <c r="D2" t="n">
-        <v>117.0</v>
+        <v>5.0</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
@@ -202,16 +202,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n" s="2">
-        <v>45649.0</v>
+        <v>45446.0</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>45825.0</v>
+        <v>45446.0</v>
       </c>
       <c r="D3" t="n">
-        <v>176.0</v>
+        <v>0.0</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -223,13 +223,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="n" s="2">
-        <v>45550.0</v>
+        <v>45378.0</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>45555.0</v>
+        <v>45378.0</v>
       </c>
       <c r="D4" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="E4" t="s">
         <v>30</v>
@@ -241,13 +241,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="n" s="2">
-        <v>45509.0</v>
+        <v>45292.0</v>
       </c>
       <c r="C5" t="n" s="2">
-        <v>45825.0</v>
+        <v>45378.0</v>
       </c>
       <c r="D5" t="n">
-        <v>316.0</v>
+        <v>86.0</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
@@ -256,13 +256,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" t="n" s="2">
-        <v>45446.0</v>
+        <v>45278.0</v>
       </c>
       <c r="C6" t="n" s="2">
-        <v>45446.0</v>
+        <v>45278.0</v>
       </c>
       <c r="D6" t="n">
         <v>0.0</v>
@@ -270,76 +270,82 @@
       <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="F6"/>
+      <c r="F6" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" t="n" s="2">
-        <v>45378.0</v>
+        <v>45183.0</v>
       </c>
       <c r="C7" t="n" s="2">
-        <v>45378.0</v>
+        <v>45184.0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="F7"/>
+      <c r="F7" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B8" t="n" s="2">
-        <v>45292.0</v>
+        <v>45118.0</v>
       </c>
       <c r="C8" t="n" s="2">
-        <v>45378.0</v>
+        <v>45233.0</v>
       </c>
       <c r="D8" t="n">
-        <v>86.0</v>
+        <v>115.0</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="F8"/>
+      <c r="F8" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9" t="n" s="2">
-        <v>45278.0</v>
+        <v>44892.0</v>
       </c>
       <c r="C9" t="n" s="2">
-        <v>45278.0</v>
+        <v>44905.0</v>
       </c>
       <c r="D9" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="n">
         <v>0.0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="n" s="2">
-        <v>45183.0</v>
+        <v>44883.0</v>
       </c>
       <c r="C10" t="n" s="2">
-        <v>45184.0</v>
+        <v>45088.0</v>
       </c>
       <c r="D10" t="n">
-        <v>1.0</v>
+        <v>205.0</v>
       </c>
       <c r="E10" t="s">
         <v>30</v>
@@ -350,96 +356,96 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B11" t="n" s="2">
-        <v>45118.0</v>
+        <v>44468.0</v>
       </c>
       <c r="C11" t="n" s="2">
-        <v>45233.0</v>
+        <v>45185.0</v>
       </c>
       <c r="D11" t="n">
-        <v>115.0</v>
+        <v>717.0</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
       </c>
       <c r="F11" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" t="n" s="2">
-        <v>44892.0</v>
+        <v>44413.0</v>
       </c>
       <c r="C12" t="n" s="2">
-        <v>44905.0</v>
+        <v>44902.0</v>
       </c>
       <c r="D12" t="n">
-        <v>13.0</v>
+        <v>489.0</v>
       </c>
       <c r="E12" t="s">
         <v>30</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B13" t="n" s="2">
-        <v>44883.0</v>
+        <v>44406.0</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>45088.0</v>
+        <v>44445.0</v>
       </c>
       <c r="D13" t="n">
-        <v>205.0</v>
+        <v>39.0</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
       </c>
       <c r="F13" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B14" t="n" s="2">
-        <v>44468.0</v>
+        <v>44255.0</v>
       </c>
       <c r="C14" t="n" s="2">
-        <v>45185.0</v>
+        <v>44291.0</v>
       </c>
       <c r="D14" t="n">
-        <v>717.0</v>
+        <v>36.0</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B15" t="n" s="2">
-        <v>44413.0</v>
+        <v>44229.0</v>
       </c>
       <c r="C15" t="n" s="2">
-        <v>44902.0</v>
+        <v>45051.0</v>
       </c>
       <c r="D15" t="n">
-        <v>489.0</v>
+        <v>822.0</v>
       </c>
       <c r="E15" t="s">
         <v>30</v>
@@ -450,42 +456,42 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B16" t="n" s="2">
-        <v>44406.0</v>
+        <v>44185.0</v>
       </c>
       <c r="C16" t="n" s="2">
-        <v>44445.0</v>
+        <v>44339.0</v>
       </c>
       <c r="D16" t="n">
-        <v>39.0</v>
+        <v>154.0</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
       </c>
       <c r="F16" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" t="n" s="2">
-        <v>44341.0</v>
+        <v>43983.0</v>
       </c>
       <c r="C17" t="n" s="2">
-        <v>45825.0</v>
+        <v>43983.0</v>
       </c>
       <c r="D17" t="n">
-        <v>1484.0</v>
+        <v>0.0</v>
       </c>
       <c r="E17" t="s">
         <v>30</v>
       </c>
       <c r="F17" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="18">
@@ -493,13 +499,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n" s="2">
-        <v>44255.0</v>
+        <v>43806.0</v>
       </c>
       <c r="C18" t="n" s="2">
-        <v>44291.0</v>
+        <v>44001.0</v>
       </c>
       <c r="D18" t="n">
-        <v>36.0</v>
+        <v>195.0</v>
       </c>
       <c r="E18" t="s">
         <v>30</v>
@@ -513,73 +519,71 @@
         <v>17</v>
       </c>
       <c r="B19" t="n" s="2">
-        <v>44229.0</v>
+        <v>43776.0</v>
       </c>
       <c r="C19" t="n" s="2">
-        <v>45051.0</v>
+        <v>43806.0</v>
       </c>
       <c r="D19" t="n">
-        <v>822.0</v>
+        <v>30.0</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2.0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B20" t="n" s="2">
-        <v>44185.0</v>
+        <v>43669.0</v>
       </c>
       <c r="C20" t="n" s="2">
-        <v>44339.0</v>
+        <v>43955.0</v>
       </c>
       <c r="D20" t="n">
-        <v>154.0</v>
+        <v>286.0</v>
       </c>
       <c r="E20" t="s">
         <v>30</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" t="n" s="2">
-        <v>43983.0</v>
+        <v>43662.0</v>
       </c>
       <c r="C21" t="n" s="2">
-        <v>43983.0</v>
+        <v>43701.0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0</v>
+        <v>39.0</v>
       </c>
       <c r="E21" t="s">
         <v>30</v>
       </c>
       <c r="F21" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" t="n" s="2">
-        <v>43806.0</v>
+        <v>43617.0</v>
       </c>
       <c r="C22" t="n" s="2">
-        <v>44001.0</v>
+        <v>43623.0</v>
       </c>
       <c r="D22" t="n">
-        <v>195.0</v>
+        <v>6.0</v>
       </c>
       <c r="E22" t="s">
         <v>30</v>
@@ -590,54 +594,56 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B23" t="n" s="2">
-        <v>43776.0</v>
+        <v>43351.0</v>
       </c>
       <c r="C23" t="n" s="2">
-        <v>43806.0</v>
+        <v>43404.0</v>
       </c>
       <c r="D23" t="n">
-        <v>30.0</v>
+        <v>53.0</v>
       </c>
       <c r="E23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23"/>
+        <v>30</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B24" t="n" s="2">
-        <v>43669.0</v>
+        <v>43347.0</v>
       </c>
       <c r="C24" t="n" s="2">
-        <v>43955.0</v>
+        <v>43457.0</v>
       </c>
       <c r="D24" t="n">
-        <v>286.0</v>
+        <v>110.0</v>
       </c>
       <c r="E24" t="s">
         <v>30</v>
       </c>
       <c r="F24" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B25" t="n" s="2">
-        <v>43662.0</v>
+        <v>43261.0</v>
       </c>
       <c r="C25" t="n" s="2">
-        <v>43701.0</v>
+        <v>43323.0</v>
       </c>
       <c r="D25" t="n">
-        <v>39.0</v>
+        <v>62.0</v>
       </c>
       <c r="E25" t="s">
         <v>30</v>
@@ -648,22 +654,22 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B26" t="n" s="2">
-        <v>43617.0</v>
+        <v>42724.0</v>
       </c>
       <c r="C26" t="n" s="2">
-        <v>43623.0</v>
+        <v>42977.0</v>
       </c>
       <c r="D26" t="n">
-        <v>6.0</v>
+        <v>253.0</v>
       </c>
       <c r="E26" t="s">
         <v>30</v>
       </c>
       <c r="F26" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="27">
@@ -671,73 +677,73 @@
         <v>17</v>
       </c>
       <c r="B27" t="n" s="2">
-        <v>43351.0</v>
+        <v>42476.0</v>
       </c>
       <c r="C27" t="n" s="2">
-        <v>43404.0</v>
+        <v>43485.0</v>
       </c>
       <c r="D27" t="n">
-        <v>53.0</v>
+        <v>1009.0</v>
       </c>
       <c r="E27" t="s">
         <v>30</v>
       </c>
       <c r="F27" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B28" t="n" s="2">
-        <v>43347.0</v>
+        <v>42456.0</v>
       </c>
       <c r="C28" t="n" s="2">
-        <v>43457.0</v>
+        <v>42581.0</v>
       </c>
       <c r="D28" t="n">
-        <v>110.0</v>
+        <v>125.0</v>
       </c>
       <c r="E28" t="s">
         <v>30</v>
       </c>
       <c r="F28" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B29" t="n" s="2">
-        <v>43261.0</v>
+        <v>41955.0</v>
       </c>
       <c r="C29" t="n" s="2">
-        <v>43323.0</v>
+        <v>41958.0</v>
       </c>
       <c r="D29" t="n">
-        <v>62.0</v>
+        <v>3.0</v>
       </c>
       <c r="E29" t="s">
         <v>30</v>
       </c>
       <c r="F29" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B30" t="n" s="2">
-        <v>42724.0</v>
+        <v>41790.0</v>
       </c>
       <c r="C30" t="n" s="2">
-        <v>42977.0</v>
+        <v>41796.0</v>
       </c>
       <c r="D30" t="n">
-        <v>253.0</v>
+        <v>6.0</v>
       </c>
       <c r="E30" t="s">
         <v>30</v>
@@ -748,56 +754,56 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B31" t="n" s="2">
-        <v>42476.0</v>
+        <v>41753.0</v>
       </c>
       <c r="C31" t="n" s="2">
-        <v>43485.0</v>
+        <v>41776.0</v>
       </c>
       <c r="D31" t="n">
-        <v>1009.0</v>
+        <v>23.0</v>
       </c>
       <c r="E31" t="s">
         <v>30</v>
       </c>
       <c r="F31" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B32" t="n" s="2">
-        <v>42456.0</v>
+        <v>41669.0</v>
       </c>
       <c r="C32" t="n" s="2">
-        <v>42581.0</v>
+        <v>42188.0</v>
       </c>
       <c r="D32" t="n">
-        <v>125.0</v>
+        <v>519.0</v>
       </c>
       <c r="E32" t="s">
         <v>30</v>
       </c>
       <c r="F32" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B33" t="n" s="2">
-        <v>41955.0</v>
+        <v>41438.0</v>
       </c>
       <c r="C33" t="n" s="2">
-        <v>41958.0</v>
+        <v>41559.0</v>
       </c>
       <c r="D33" t="n">
-        <v>3.0</v>
+        <v>121.0</v>
       </c>
       <c r="E33" t="s">
         <v>30</v>
@@ -811,13 +817,13 @@
         <v>13</v>
       </c>
       <c r="B34" t="n" s="2">
-        <v>41790.0</v>
+        <v>41407.0</v>
       </c>
       <c r="C34" t="n" s="2">
-        <v>41796.0</v>
+        <v>41451.0</v>
       </c>
       <c r="D34" t="n">
-        <v>6.0</v>
+        <v>44.0</v>
       </c>
       <c r="E34" t="s">
         <v>30</v>
@@ -828,136 +834,134 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B35" t="n" s="2">
-        <v>41753.0</v>
+        <v>41318.0</v>
       </c>
       <c r="C35" t="n" s="2">
-        <v>41776.0</v>
+        <v>42339.0</v>
       </c>
       <c r="D35" t="n">
-        <v>23.0</v>
+        <v>1021.0</v>
       </c>
       <c r="E35" t="s">
         <v>30</v>
       </c>
       <c r="F35" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B36" t="n" s="2">
-        <v>41669.0</v>
+        <v>41100.0</v>
       </c>
       <c r="C36" t="n" s="2">
-        <v>42188.0</v>
+        <v>41100.0</v>
       </c>
       <c r="D36" t="n">
-        <v>519.0</v>
+        <v>0.0</v>
       </c>
       <c r="E36" t="s">
         <v>30</v>
       </c>
       <c r="F36" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B37" t="n" s="2">
-        <v>41438.0</v>
+        <v>40957.0</v>
       </c>
       <c r="C37" t="n" s="2">
-        <v>41559.0</v>
+        <v>40957.0</v>
       </c>
       <c r="D37" t="n">
-        <v>121.0</v>
+        <v>0.0</v>
       </c>
       <c r="E37" t="s">
         <v>30</v>
       </c>
       <c r="F37" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B38" t="n" s="2">
-        <v>41407.0</v>
+        <v>40743.0</v>
       </c>
       <c r="C38" t="n" s="2">
-        <v>41451.0</v>
+        <v>42234.0</v>
       </c>
       <c r="D38" t="n">
-        <v>44.0</v>
+        <v>1491.0</v>
       </c>
       <c r="E38" t="s">
         <v>30</v>
       </c>
       <c r="F38" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B39" t="n" s="2">
-        <v>41318.0</v>
+        <v>40656.0</v>
       </c>
       <c r="C39" t="n" s="2">
-        <v>42339.0</v>
+        <v>40787.0</v>
       </c>
       <c r="D39" t="n">
-        <v>1021.0</v>
+        <v>131.0</v>
       </c>
       <c r="E39" t="s">
         <v>30</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B40" t="n" s="2">
-        <v>41100.0</v>
+        <v>40432.0</v>
       </c>
       <c r="C40" t="n" s="2">
-        <v>41100.0</v>
+        <v>40433.0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E40" t="s">
-        <v>30</v>
-      </c>
-      <c r="F40" t="n">
-        <v>2.0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B41" t="n" s="2">
-        <v>40957.0</v>
+        <v>40328.0</v>
       </c>
       <c r="C41" t="n" s="2">
-        <v>40957.0</v>
+        <v>40331.0</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="E41" t="s">
         <v>30</v>
@@ -968,22 +972,22 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B42" t="n" s="2">
-        <v>40743.0</v>
+        <v>40325.0</v>
       </c>
       <c r="C42" t="n" s="2">
-        <v>42234.0</v>
+        <v>40327.0</v>
       </c>
       <c r="D42" t="n">
-        <v>1491.0</v>
+        <v>2.0</v>
       </c>
       <c r="E42" t="s">
         <v>30</v>
       </c>
       <c r="F42" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="43">
@@ -991,51 +995,53 @@
         <v>14</v>
       </c>
       <c r="B43" t="n" s="2">
-        <v>40656.0</v>
+        <v>40301.0</v>
       </c>
       <c r="C43" t="n" s="2">
-        <v>40787.0</v>
+        <v>40401.0</v>
       </c>
       <c r="D43" t="n">
-        <v>131.0</v>
+        <v>100.0</v>
       </c>
       <c r="E43" t="s">
         <v>30</v>
       </c>
       <c r="F43" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44" t="n" s="2">
-        <v>40432.0</v>
+        <v>40088.0</v>
       </c>
       <c r="C44" t="n" s="2">
-        <v>40433.0</v>
+        <v>40159.0</v>
       </c>
       <c r="D44" t="n">
-        <v>1.0</v>
+        <v>71.0</v>
       </c>
       <c r="E44" t="s">
-        <v>31</v>
-      </c>
-      <c r="F44"/>
+        <v>30</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B45" t="n" s="2">
-        <v>40328.0</v>
+        <v>39989.0</v>
       </c>
       <c r="C45" t="n" s="2">
-        <v>40331.0</v>
+        <v>39989.0</v>
       </c>
       <c r="D45" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E45" t="s">
         <v>30</v>
@@ -1046,16 +1052,16 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B46" t="n" s="2">
-        <v>40325.0</v>
+        <v>39887.0</v>
       </c>
       <c r="C46" t="n" s="2">
-        <v>40327.0</v>
+        <v>39995.0</v>
       </c>
       <c r="D46" t="n">
-        <v>2.0</v>
+        <v>108.0</v>
       </c>
       <c r="E46" t="s">
         <v>30</v>
@@ -1066,214 +1072,214 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B47" t="n" s="2">
-        <v>40301.0</v>
+        <v>39815.0</v>
       </c>
       <c r="C47" t="n" s="2">
-        <v>40401.0</v>
+        <v>39834.0</v>
       </c>
       <c r="D47" t="n">
-        <v>100.0</v>
+        <v>19.0</v>
       </c>
       <c r="E47" t="s">
         <v>30</v>
       </c>
       <c r="F47" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B48" t="n" s="2">
-        <v>40088.0</v>
+        <v>39667.0</v>
       </c>
       <c r="C48" t="n" s="2">
-        <v>40159.0</v>
+        <v>39669.0</v>
       </c>
       <c r="D48" t="n">
-        <v>71.0</v>
+        <v>2.0</v>
       </c>
       <c r="E48" t="s">
         <v>30</v>
       </c>
       <c r="F48" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B49" t="n" s="2">
-        <v>39989.0</v>
+        <v>39641.0</v>
       </c>
       <c r="C49" t="n" s="2">
-        <v>39989.0</v>
+        <v>39679.0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.0</v>
+        <v>38.0</v>
       </c>
       <c r="E49" t="s">
         <v>30</v>
       </c>
       <c r="F49" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B50" t="n" s="2">
-        <v>39887.0</v>
+        <v>39500.0</v>
       </c>
       <c r="C50" t="n" s="2">
-        <v>39995.0</v>
+        <v>39508.0</v>
       </c>
       <c r="D50" t="n">
-        <v>108.0</v>
+        <v>8.0</v>
       </c>
       <c r="E50" t="s">
         <v>30</v>
       </c>
       <c r="F50" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B51" t="n" s="2">
-        <v>39815.0</v>
+        <v>39490.0</v>
       </c>
       <c r="C51" t="n" s="2">
-        <v>39834.0</v>
+        <v>39490.0</v>
       </c>
       <c r="D51" t="n">
-        <v>19.0</v>
+        <v>0.0</v>
       </c>
       <c r="E51" t="s">
-        <v>30</v>
-      </c>
-      <c r="F51" t="n">
-        <v>2.0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B52" t="n" s="2">
-        <v>39667.0</v>
+        <v>39413.0</v>
       </c>
       <c r="C52" t="n" s="2">
         <v>39669.0</v>
       </c>
       <c r="D52" t="n">
-        <v>2.0</v>
+        <v>256.0</v>
       </c>
       <c r="E52" t="s">
         <v>30</v>
       </c>
       <c r="F52" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B53" t="n" s="2">
-        <v>39641.0</v>
+        <v>39309.0</v>
       </c>
       <c r="C53" t="n" s="2">
-        <v>39679.0</v>
+        <v>39338.0</v>
       </c>
       <c r="D53" t="n">
-        <v>38.0</v>
+        <v>29.0</v>
       </c>
       <c r="E53" t="s">
         <v>30</v>
       </c>
       <c r="F53" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B54" t="n" s="2">
-        <v>39500.0</v>
+        <v>39250.0</v>
       </c>
       <c r="C54" t="n" s="2">
-        <v>39508.0</v>
+        <v>39672.0</v>
       </c>
       <c r="D54" t="n">
-        <v>8.0</v>
+        <v>422.0</v>
       </c>
       <c r="E54" t="s">
         <v>30</v>
       </c>
       <c r="F54" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B55" t="n" s="2">
-        <v>39490.0</v>
+        <v>39055.0</v>
       </c>
       <c r="C55" t="n" s="2">
-        <v>39490.0</v>
+        <v>39059.0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="E55" t="s">
-        <v>31</v>
-      </c>
-      <c r="F55"/>
+        <v>30</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B56" t="n" s="2">
-        <v>39413.0</v>
+        <v>39046.0</v>
       </c>
       <c r="C56" t="n" s="2">
-        <v>39669.0</v>
+        <v>39144.0</v>
       </c>
       <c r="D56" t="n">
-        <v>256.0</v>
+        <v>98.0</v>
       </c>
       <c r="E56" t="s">
         <v>30</v>
       </c>
       <c r="F56" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B57" t="n" s="2">
-        <v>39309.0</v>
+        <v>38977.0</v>
       </c>
       <c r="C57" t="n" s="2">
-        <v>39338.0</v>
+        <v>38977.0</v>
       </c>
       <c r="D57" t="n">
-        <v>29.0</v>
+        <v>0.0</v>
       </c>
       <c r="E57" t="s">
         <v>30</v>
@@ -1284,16 +1290,16 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B58" t="n" s="2">
-        <v>39250.0</v>
+        <v>38796.0</v>
       </c>
       <c r="C58" t="n" s="2">
-        <v>39672.0</v>
+        <v>38894.0</v>
       </c>
       <c r="D58" t="n">
-        <v>422.0</v>
+        <v>98.0</v>
       </c>
       <c r="E58" t="s">
         <v>30</v>
@@ -1304,16 +1310,16 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B59" t="n" s="2">
-        <v>39055.0</v>
+        <v>38779.0</v>
       </c>
       <c r="C59" t="n" s="2">
-        <v>39059.0</v>
+        <v>38967.0</v>
       </c>
       <c r="D59" t="n">
-        <v>4.0</v>
+        <v>188.0</v>
       </c>
       <c r="E59" t="s">
         <v>30</v>
@@ -1324,196 +1330,196 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B60" t="n" s="2">
-        <v>39046.0</v>
+        <v>38754.0</v>
       </c>
       <c r="C60" t="n" s="2">
-        <v>39144.0</v>
+        <v>39018.0</v>
       </c>
       <c r="D60" t="n">
-        <v>98.0</v>
+        <v>264.0</v>
       </c>
       <c r="E60" t="s">
         <v>30</v>
       </c>
       <c r="F60" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B61" t="n" s="2">
-        <v>38977.0</v>
+        <v>38695.0</v>
       </c>
       <c r="C61" t="n" s="2">
-        <v>38977.0</v>
+        <v>38834.0</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0</v>
+        <v>139.0</v>
       </c>
       <c r="E61" t="s">
         <v>30</v>
       </c>
       <c r="F61" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B62" t="n" s="2">
-        <v>38796.0</v>
+        <v>38602.0</v>
       </c>
       <c r="C62" t="n" s="2">
-        <v>38894.0</v>
+        <v>38660.0</v>
       </c>
       <c r="D62" t="n">
-        <v>98.0</v>
+        <v>58.0</v>
       </c>
       <c r="E62" t="s">
         <v>30</v>
       </c>
       <c r="F62" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B63" t="n" s="2">
-        <v>38779.0</v>
+        <v>38424.0</v>
       </c>
       <c r="C63" t="n" s="2">
-        <v>38967.0</v>
+        <v>38683.0</v>
       </c>
       <c r="D63" t="n">
-        <v>188.0</v>
+        <v>259.0</v>
       </c>
       <c r="E63" t="s">
         <v>30</v>
       </c>
       <c r="F63" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B64" t="n" s="2">
-        <v>38754.0</v>
+        <v>38406.0</v>
       </c>
       <c r="C64" t="n" s="2">
-        <v>39018.0</v>
+        <v>38477.0</v>
       </c>
       <c r="D64" t="n">
-        <v>264.0</v>
+        <v>71.0</v>
       </c>
       <c r="E64" t="s">
         <v>30</v>
       </c>
       <c r="F64" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B65" t="n" s="2">
-        <v>38695.0</v>
+        <v>38356.0</v>
       </c>
       <c r="C65" t="n" s="2">
-        <v>38834.0</v>
+        <v>38397.0</v>
       </c>
       <c r="D65" t="n">
-        <v>139.0</v>
+        <v>41.0</v>
       </c>
       <c r="E65" t="s">
         <v>30</v>
       </c>
       <c r="F65" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B66" t="n" s="2">
-        <v>38602.0</v>
+        <v>38261.0</v>
       </c>
       <c r="C66" t="n" s="2">
-        <v>38660.0</v>
+        <v>39474.0</v>
       </c>
       <c r="D66" t="n">
-        <v>58.0</v>
+        <v>1213.0</v>
       </c>
       <c r="E66" t="s">
         <v>30</v>
       </c>
       <c r="F66" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B67" t="n" s="2">
-        <v>38424.0</v>
+        <v>38161.0</v>
       </c>
       <c r="C67" t="n" s="2">
-        <v>38683.0</v>
+        <v>38172.0</v>
       </c>
       <c r="D67" t="n">
-        <v>259.0</v>
+        <v>11.0</v>
       </c>
       <c r="E67" t="s">
         <v>30</v>
       </c>
       <c r="F67" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B68" t="n" s="2">
-        <v>38406.0</v>
+        <v>38089.0</v>
       </c>
       <c r="C68" t="n" s="2">
-        <v>38477.0</v>
+        <v>38598.0</v>
       </c>
       <c r="D68" t="n">
-        <v>71.0</v>
+        <v>509.0</v>
       </c>
       <c r="E68" t="s">
         <v>30</v>
       </c>
       <c r="F68" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B69" t="n" s="2">
-        <v>38356.0</v>
+        <v>38034.0</v>
       </c>
       <c r="C69" t="n" s="2">
-        <v>38397.0</v>
+        <v>38184.0</v>
       </c>
       <c r="D69" t="n">
-        <v>41.0</v>
+        <v>150.0</v>
       </c>
       <c r="E69" t="s">
         <v>30</v>
@@ -1524,16 +1530,16 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B70" t="n" s="2">
-        <v>38261.0</v>
+        <v>38033.0</v>
       </c>
       <c r="C70" t="n" s="2">
-        <v>39474.0</v>
+        <v>38235.0</v>
       </c>
       <c r="D70" t="n">
-        <v>1213.0</v>
+        <v>202.0</v>
       </c>
       <c r="E70" t="s">
         <v>30</v>
@@ -1544,199 +1550,119 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B71" t="n" s="2">
-        <v>38161.0</v>
+        <v>37751.0</v>
       </c>
       <c r="C71" t="n" s="2">
-        <v>38172.0</v>
+        <v>37814.0</v>
       </c>
       <c r="D71" t="n">
-        <v>11.0</v>
+        <v>63.0</v>
       </c>
       <c r="E71" t="s">
         <v>30</v>
       </c>
       <c r="F71" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B72" t="n" s="2">
-        <v>38089.0</v>
+        <v>37523.0</v>
       </c>
       <c r="C72" t="n" s="2">
-        <v>38598.0</v>
+        <v>37703.0</v>
       </c>
       <c r="D72" t="n">
-        <v>509.0</v>
+        <v>180.0</v>
       </c>
       <c r="E72" t="s">
         <v>30</v>
       </c>
       <c r="F72" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B73" t="n" s="2">
-        <v>38034.0</v>
+        <v>37469.0</v>
       </c>
       <c r="C73" t="n" s="2">
-        <v>38184.0</v>
+        <v>37470.0</v>
       </c>
       <c r="D73" t="n">
-        <v>150.0</v>
+        <v>1.0</v>
       </c>
       <c r="E73" t="s">
-        <v>30</v>
-      </c>
-      <c r="F73" t="n">
-        <v>2.0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F73"/>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B74" t="n" s="2">
-        <v>38033.0</v>
+        <v>37431.0</v>
       </c>
       <c r="C74" t="n" s="2">
-        <v>38235.0</v>
+        <v>37442.0</v>
       </c>
       <c r="D74" t="n">
-        <v>202.0</v>
+        <v>11.0</v>
       </c>
       <c r="E74" t="s">
         <v>30</v>
       </c>
       <c r="F74" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B75" t="n" s="2">
-        <v>37751.0</v>
+        <v>37005.0</v>
       </c>
       <c r="C75" t="n" s="2">
-        <v>37814.0</v>
+        <v>37006.0</v>
       </c>
       <c r="D75" t="n">
-        <v>63.0</v>
+        <v>1.0</v>
       </c>
       <c r="E75" t="s">
         <v>30</v>
       </c>
       <c r="F75" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B76" t="n" s="2">
-        <v>37523.0</v>
+        <v>36924.0</v>
       </c>
       <c r="C76" t="n" s="2">
-        <v>37703.0</v>
+        <v>36996.0</v>
       </c>
       <c r="D76" t="n">
-        <v>180.0</v>
+        <v>72.0</v>
       </c>
       <c r="E76" t="s">
         <v>30</v>
       </c>
       <c r="F76" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>29</v>
-      </c>
-      <c r="B77" t="n" s="2">
-        <v>37469.0</v>
-      </c>
-      <c r="C77" t="n" s="2">
-        <v>37470.0</v>
-      </c>
-      <c r="D77" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E77" t="s">
-        <v>31</v>
-      </c>
-      <c r="F77"/>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
-        <v>6</v>
-      </c>
-      <c r="B78" t="n" s="2">
-        <v>37431.0</v>
-      </c>
-      <c r="C78" t="n" s="2">
-        <v>37442.0</v>
-      </c>
-      <c r="D78" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="E78" t="s">
-        <v>30</v>
-      </c>
-      <c r="F78" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s">
-        <v>8</v>
-      </c>
-      <c r="B79" t="n" s="2">
-        <v>37005.0</v>
-      </c>
-      <c r="C79" t="n" s="2">
-        <v>37006.0</v>
-      </c>
-      <c r="D79" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E79" t="s">
-        <v>30</v>
-      </c>
-      <c r="F79" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s">
-        <v>18</v>
-      </c>
-      <c r="B80" t="n" s="2">
-        <v>36924.0</v>
-      </c>
-      <c r="C80" t="n" s="2">
-        <v>36996.0</v>
-      </c>
-      <c r="D80" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="E80" t="s">
-        <v>30</v>
-      </c>
-      <c r="F80" t="n">
         <v>3.0</v>
       </c>
     </row>

</xml_diff>